<commit_message>
Created new test script to work on Multiple Windows in HeroKUApp
</commit_message>
<xml_diff>
--- a/target/classes/Module9_TestNG/DataDriver/DataDriver_IFrame_TinyMCE_WYSIWYG_Editor.xlsx
+++ b/target/classes/Module9_TestNG/DataDriver/DataDriver_IFrame_TinyMCE_WYSIWYG_Editor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ashish\Training\Selenium\Web Driver\SeleniumTraining_AshishThakur\src\Module9_TestNG\DataDriver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807280CB-C487-4498-8A47-12CD189D7273}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E051E9-6F30-4D38-951E-5A36B4899C1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="72" windowWidth="20112" windowHeight="7992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,9 +55,6 @@
     <t>TC4</t>
   </si>
   <si>
-    <t>B;Justify;Align Right;Decrease-Indent;I</t>
-  </si>
-  <si>
     <t>Bullet-List;I;Align-center;Align-left;Align-right</t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t>Bold;Italic;Justify;right;Increase indent</t>
+  </si>
+  <si>
+    <t>Bold;Justify;right;Decrease-indent;Italic</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,10 +515,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -529,10 +529,10 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -543,10 +543,10 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -557,10 +557,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -590,7 +590,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -601,7 +601,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -612,7 +612,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -641,7 +641,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -652,7 +652,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -663,7 +663,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -693,7 +693,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -704,7 +704,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -715,7 +715,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>